<commit_message>
Updated map and calculator
</commit_message>
<xml_diff>
--- a/raw-data/Regional Data - Timeseries.xlsx
+++ b/raw-data/Regional Data - Timeseries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\OneDrive\Documents\PyCharm\Projects\Sarah C Gall Ltd\Clients\ASI\ASI Housing Freedom Day\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A0EAAE-A11F-4D67-B634-9033F37B7C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03EABEE-D4DB-49A6-940D-714AED1447D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4150" yWindow="2980" windowWidth="22700" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4150" yWindow="2980" windowWidth="22700" windowHeight="14480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeseries" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1560" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="779">
   <si>
     <t>Region</t>
   </si>
@@ -2373,6 +2373,9 @@
   </si>
   <si>
     <t>Population</t>
+  </si>
+  <si>
+    <t>Change</t>
   </si>
 </sst>
 </file>
@@ -2977,6 +2980,1532 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Housing Supply'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dwellings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Housing Supply'!$A$2:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Housing Supply'!$B$2:$B$53</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>272520</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>249710</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>229360</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>261460</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>263430</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>261600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>241360</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>209460</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>204370</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>170600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>151630</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>173720</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>182080</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>170040</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>179140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>189300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>202930</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>179360</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>163900</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>154600</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>143830</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>147840</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>154640</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>157140</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>149090</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>149490</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>142650</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>141010</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>135100</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>129510</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>136800</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>144060</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>154070</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>159450</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>160850</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>176650</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>148010</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>124970</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>106720</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>114020</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>115590</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>109440</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>117810</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>142470</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>141870</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>162480</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>165490</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>177880</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>146650</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>174950</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>178010</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2AF1-427D-9761-A4D5058E0DB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Housing Supply'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Change</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Housing Supply'!$A$2:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1972</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1974</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1978</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1979</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1980</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1981</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1983</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1984</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1985</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1986</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1987</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Housing Supply'!$D$2:$D$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>160200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-8300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-14500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-20100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59900</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-43500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36400</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>98700</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>145000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>130200</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>112800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>111900</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>140400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>146400</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>175900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>123000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>104300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>126500</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>154700</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>135600</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>145700</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>155800</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>212300</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>200400</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>216400</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>229600</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>246200</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>269100</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>411400</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>359200</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>415900</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>434800</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>380500</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>446100</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>464700</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>399600</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>411900</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>451600</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>438400</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>480300</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>330500</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>305000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>305600</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95900</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>228900</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>551500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2AF1-427D-9761-A4D5058E0DB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="362572000"/>
+        <c:axId val="362572480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="362572000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362572480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="362572480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="362572000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>111124</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B76F53-F04D-8996-AA96-6AD6C4ABDBB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3296,7 +4825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -3369,7 +4898,7 @@
         <v>495</v>
       </c>
       <c r="D2" s="1">
-        <f>(C2*12)/B2</f>
+        <f t="shared" ref="D2:D11" si="0">(C2*12)/B2</f>
         <v>0.26268075885552561</v>
       </c>
       <c r="E2">
@@ -3382,38 +4911,38 @@
         <v>550</v>
       </c>
       <c r="H2" s="1">
-        <f>(G2*12)/F2</f>
+        <f t="shared" ref="H2:H11" si="1">(G2*12)/F2</f>
         <v>0.24481620238139395</v>
       </c>
       <c r="I2">
         <v>89.419117920000005</v>
       </c>
       <c r="J2">
-        <f>F2-B2</f>
+        <f t="shared" ref="J2:J11" si="2">F2-B2</f>
         <v>4346</v>
       </c>
       <c r="K2">
-        <f>G2-C2</f>
+        <f t="shared" ref="K2:K11" si="3">G2-C2</f>
         <v>55</v>
       </c>
       <c r="L2" s="1">
-        <f>H2-D2</f>
+        <f t="shared" ref="L2:L11" si="4">H2-D2</f>
         <v>-1.7864556474131654E-2</v>
       </c>
       <c r="M2" s="2">
-        <f>I2-E2</f>
+        <f t="shared" ref="M2:M11" si="5">I2-E2</f>
         <v>-6.5250292499999887</v>
       </c>
       <c r="N2" s="6">
-        <f>J2/F2</f>
+        <f t="shared" ref="N2:N11" si="6">J2/F2</f>
         <v>0.16120775993174821</v>
       </c>
       <c r="O2" s="6">
-        <f>K2/G2</f>
+        <f t="shared" ref="O2:O11" si="7">K2/G2</f>
         <v>0.1</v>
       </c>
       <c r="P2" s="6">
-        <f>N2-O2</f>
+        <f t="shared" ref="P2:P11" si="8">N2-O2</f>
         <v>6.1207759931748207E-2</v>
       </c>
     </row>
@@ -3428,7 +4957,7 @@
         <v>725</v>
       </c>
       <c r="D3" s="1">
-        <f>(C3*12)/B3</f>
+        <f t="shared" si="0"/>
         <v>0.37470927728486519</v>
       </c>
       <c r="E3">
@@ -3441,38 +4970,38 @@
         <v>850</v>
       </c>
       <c r="H3" s="1">
-        <f>(G3*12)/F3</f>
+        <f t="shared" si="1"/>
         <v>0.35480729094197855</v>
       </c>
       <c r="I3">
         <v>129.59336300000001</v>
       </c>
       <c r="J3">
-        <f>F3-B3</f>
+        <f t="shared" si="2"/>
         <v>5530</v>
       </c>
       <c r="K3">
-        <f>G3-C3</f>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="L3" s="1">
-        <f>H3-D3</f>
+        <f t="shared" si="4"/>
         <v>-1.9901986342886646E-2</v>
       </c>
       <c r="M3" s="2">
-        <f>I3-E3</f>
+        <f t="shared" si="5"/>
         <v>-7.2692004999999824</v>
       </c>
       <c r="N3" s="6">
-        <f>J3/F3</f>
+        <f t="shared" si="6"/>
         <v>0.19236120773619034</v>
       </c>
       <c r="O3" s="6">
-        <f>K3/G3</f>
+        <f t="shared" si="7"/>
         <v>0.14705882352941177</v>
       </c>
       <c r="P3" s="6">
-        <f>N3-O3</f>
+        <f t="shared" si="8"/>
         <v>4.5302384206778568E-2</v>
       </c>
     </row>
@@ -3487,7 +5016,7 @@
         <v>1450</v>
       </c>
       <c r="D4" s="1">
-        <f>(C4*12)/B4</f>
+        <f t="shared" si="0"/>
         <v>0.55753148130347019</v>
       </c>
       <c r="E4">
@@ -3500,38 +5029,38 @@
         <v>1625</v>
       </c>
       <c r="H4" s="1">
-        <f>(G4*12)/F4</f>
+        <f t="shared" si="1"/>
         <v>0.53891222639840819</v>
       </c>
       <c r="I4">
         <v>196.8376907</v>
       </c>
       <c r="J4">
-        <f>F4-B4</f>
+        <f t="shared" si="2"/>
         <v>4975</v>
       </c>
       <c r="K4">
-        <f>G4-C4</f>
+        <f t="shared" si="3"/>
         <v>175</v>
       </c>
       <c r="L4" s="1">
-        <f>H4-D4</f>
+        <f t="shared" si="4"/>
         <v>-1.8619254905061999E-2</v>
       </c>
       <c r="M4" s="2">
-        <f>I4-E4</f>
+        <f t="shared" si="5"/>
         <v>-6.8006828000000041</v>
       </c>
       <c r="N4" s="6">
-        <f>J4/F4</f>
+        <f t="shared" si="6"/>
         <v>0.1374917090426708</v>
       </c>
       <c r="O4" s="6">
-        <f>K4/G4</f>
+        <f t="shared" si="7"/>
         <v>0.1076923076923077</v>
       </c>
       <c r="P4" s="6">
-        <f>N4-O4</f>
+        <f t="shared" si="8"/>
         <v>2.9799401350363103E-2</v>
       </c>
     </row>
@@ -3546,7 +5075,7 @@
         <v>550</v>
       </c>
       <c r="D5" s="1">
-        <f>(C5*12)/B5</f>
+        <f t="shared" si="0"/>
         <v>0.28693157116772455</v>
       </c>
       <c r="E5">
@@ -3559,38 +5088,38 @@
         <v>650</v>
       </c>
       <c r="H5" s="1">
-        <f>(G5*12)/F5</f>
+        <f t="shared" si="1"/>
         <v>0.28211805555555558</v>
       </c>
       <c r="I5">
         <v>103.0436198</v>
       </c>
       <c r="J5">
-        <f>F5-B5</f>
+        <f t="shared" si="2"/>
         <v>4646</v>
       </c>
       <c r="K5">
-        <f>G5-C5</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="L5" s="1">
-        <f>H5-D5</f>
+        <f t="shared" si="4"/>
         <v>-4.8135156121689726E-3</v>
       </c>
       <c r="M5" s="2">
-        <f>I5-E5</f>
+        <f t="shared" si="5"/>
         <v>-1.7581366000000003</v>
       </c>
       <c r="N5" s="6">
-        <f>J5/F5</f>
+        <f t="shared" si="6"/>
         <v>0.16804108796296297</v>
       </c>
       <c r="O5" s="6">
-        <f>K5/G5</f>
+        <f t="shared" si="7"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="P5" s="6">
-        <f>N5-O5</f>
+        <f t="shared" si="8"/>
         <v>1.419493411680911E-2</v>
       </c>
     </row>
@@ -3605,7 +5134,7 @@
         <v>795</v>
       </c>
       <c r="D6" s="1">
-        <f>(C6*12)/B6</f>
+        <f t="shared" si="0"/>
         <v>0.36589575422851223</v>
       </c>
       <c r="E6">
@@ -3618,38 +5147,38 @@
         <v>925</v>
       </c>
       <c r="H6" s="1">
-        <f>(G6*12)/F6</f>
+        <f t="shared" si="1"/>
         <v>0.36041301383206703</v>
       </c>
       <c r="I6">
         <v>131.6408533</v>
       </c>
       <c r="J6">
-        <f>F6-B6</f>
+        <f t="shared" si="2"/>
         <v>4725</v>
       </c>
       <c r="K6">
-        <f>G6-C6</f>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="L6" s="1">
-        <f>H6-D6</f>
+        <f t="shared" si="4"/>
         <v>-5.482740396445196E-3</v>
       </c>
       <c r="M6" s="2">
-        <f>I6-E6</f>
+        <f t="shared" si="5"/>
         <v>-2.0025708999999949</v>
       </c>
       <c r="N6" s="6">
-        <f>J6/F6</f>
+        <f t="shared" si="6"/>
         <v>0.15341905318527177</v>
       </c>
       <c r="O6" s="6">
-        <f>K6/G6</f>
+        <f t="shared" si="7"/>
         <v>0.14054054054054055</v>
       </c>
       <c r="P6" s="6">
-        <f>N6-O6</f>
+        <f t="shared" si="8"/>
         <v>1.2878512644731221E-2</v>
       </c>
     </row>
@@ -3664,7 +5193,7 @@
         <v>565</v>
       </c>
       <c r="D7" s="1">
-        <f>(C7*12)/B7</f>
+        <f t="shared" si="0"/>
         <v>0.28558190472178929</v>
       </c>
       <c r="E7">
@@ -3677,38 +5206,38 @@
         <v>675</v>
       </c>
       <c r="H7" s="1">
-        <f>(G7*12)/F7</f>
+        <f t="shared" si="1"/>
         <v>0.28492032783425375</v>
       </c>
       <c r="I7">
         <v>104.0671497</v>
       </c>
       <c r="J7">
-        <f>F7-B7</f>
+        <f t="shared" si="2"/>
         <v>4688</v>
       </c>
       <c r="K7">
-        <f>G7-C7</f>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="L7" s="1">
-        <f>H7-D7</f>
+        <f t="shared" si="4"/>
         <v>-6.6157688753554211E-4</v>
       </c>
       <c r="M7" s="2">
-        <f>I7-E7</f>
+        <f t="shared" si="5"/>
         <v>-0.24164100000000133</v>
       </c>
       <c r="N7" s="6">
-        <f>J7/F7</f>
+        <f t="shared" si="6"/>
         <v>0.16490203665271377</v>
       </c>
       <c r="O7" s="6">
-        <f>K7/G7</f>
+        <f t="shared" si="7"/>
         <v>0.16296296296296298</v>
       </c>
       <c r="P7" s="6">
-        <f>N7-O7</f>
+        <f t="shared" si="8"/>
         <v>1.9390736897507976E-3</v>
       </c>
     </row>
@@ -3723,7 +5252,7 @@
         <v>595</v>
       </c>
       <c r="D8" s="1">
-        <f>(C8*12)/B8</f>
+        <f t="shared" si="0"/>
         <v>0.3023502011433411</v>
       </c>
       <c r="E8">
@@ -3736,38 +5265,38 @@
         <v>700</v>
       </c>
       <c r="H8" s="1">
-        <f>(G8*12)/F8</f>
+        <f t="shared" si="1"/>
         <v>0.30235404218558781</v>
       </c>
       <c r="I8">
         <v>110.43481389999999</v>
       </c>
       <c r="J8">
-        <f>F8-B8</f>
+        <f t="shared" si="2"/>
         <v>4167</v>
       </c>
       <c r="K8">
-        <f>G8-C8</f>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="L8" s="1">
-        <f>H8-D8</f>
+        <f t="shared" si="4"/>
         <v>3.8410422467105576E-6</v>
       </c>
       <c r="M8" s="2">
-        <f>I8-E8</f>
+        <f t="shared" si="5"/>
         <v>1.4028999999879943E-3</v>
       </c>
       <c r="N8" s="6">
-        <f>J8/F8</f>
+        <f t="shared" si="6"/>
         <v>0.14998920164135052</v>
       </c>
       <c r="O8" s="6">
-        <f>K8/G8</f>
+        <f t="shared" si="7"/>
         <v>0.15</v>
       </c>
       <c r="P8" s="6">
-        <f>N8-O8</f>
+        <f t="shared" si="8"/>
         <v>-1.0798358649477535E-5</v>
       </c>
     </row>
@@ -3782,7 +5311,7 @@
         <v>625</v>
       </c>
       <c r="D9" s="1">
-        <f>(C9*12)/B9</f>
+        <f t="shared" si="0"/>
         <v>0.31736628300609343</v>
       </c>
       <c r="E9">
@@ -3795,38 +5324,38 @@
         <v>750</v>
       </c>
       <c r="H9" s="1">
-        <f>(G9*12)/F9</f>
+        <f t="shared" si="1"/>
         <v>0.31743792325056436</v>
       </c>
       <c r="I9">
         <v>115.94420150000001</v>
       </c>
       <c r="J9">
-        <f>F9-B9</f>
+        <f t="shared" si="2"/>
         <v>4720</v>
       </c>
       <c r="K9">
-        <f>G9-C9</f>
+        <f t="shared" si="3"/>
         <v>125</v>
       </c>
       <c r="L9" s="1">
-        <f>H9-D9</f>
+        <f t="shared" si="4"/>
         <v>7.1640244470927428E-5</v>
       </c>
       <c r="M9" s="2">
-        <f>I9-E9</f>
+        <f t="shared" si="5"/>
         <v>2.6166600000010476E-2</v>
       </c>
       <c r="N9" s="6">
-        <f>J9/F9</f>
+        <f t="shared" si="6"/>
         <v>0.1664785553047404</v>
       </c>
       <c r="O9" s="6">
-        <f>K9/G9</f>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="P9" s="6">
-        <f>N9-O9</f>
+        <f t="shared" si="8"/>
         <v>-1.8811136192625755E-4</v>
       </c>
     </row>
@@ -3841,7 +5370,7 @@
         <v>895</v>
       </c>
       <c r="D10" s="1">
-        <f>(C10*12)/B10</f>
+        <f t="shared" si="0"/>
         <v>0.39572586588061903</v>
       </c>
       <c r="E10">
@@ -3854,38 +5383,38 @@
         <v>1050</v>
       </c>
       <c r="H10" s="1">
-        <f>(G10*12)/F10</f>
+        <f t="shared" si="1"/>
         <v>0.39622641509433965</v>
       </c>
       <c r="I10">
         <v>144.7216981</v>
       </c>
       <c r="J10">
-        <f>F10-B10</f>
+        <f t="shared" si="2"/>
         <v>4660</v>
       </c>
       <c r="K10">
-        <f>G10-C10</f>
+        <f t="shared" si="3"/>
         <v>155</v>
       </c>
       <c r="L10" s="1">
-        <f>H10-D10</f>
+        <f t="shared" si="4"/>
         <v>5.0054921372061356E-4</v>
       </c>
       <c r="M10" s="2">
-        <f>I10-E10</f>
+        <f t="shared" si="5"/>
         <v>0.18282560000000103</v>
       </c>
       <c r="N10" s="6">
-        <f>J10/F10</f>
+        <f t="shared" si="6"/>
         <v>0.14654088050314465</v>
       </c>
       <c r="O10" s="6">
-        <f>K10/G10</f>
+        <f t="shared" si="7"/>
         <v>0.14761904761904762</v>
       </c>
       <c r="P10" s="6">
-        <f>N10-O10</f>
+        <f t="shared" si="8"/>
         <v>-1.0781671159029727E-3</v>
       </c>
     </row>
@@ -3900,7 +5429,7 @@
         <v>700</v>
       </c>
       <c r="D11" s="1">
-        <f>(C11*12)/B11</f>
+        <f t="shared" si="0"/>
         <v>0.33399602385685884</v>
       </c>
       <c r="E11">
@@ -3913,38 +5442,38 @@
         <v>850</v>
       </c>
       <c r="H11" s="1">
-        <f>(G11*12)/F11</f>
+        <f t="shared" si="1"/>
         <v>0.34092048531033792</v>
       </c>
       <c r="I11">
         <v>124.5212073</v>
       </c>
       <c r="J11">
-        <f>F11-B11</f>
+        <f t="shared" si="2"/>
         <v>4769</v>
       </c>
       <c r="K11">
-        <f>G11-C11</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="L11" s="1">
-        <f>H11-D11</f>
+        <f t="shared" si="4"/>
         <v>6.9244614534790805E-3</v>
       </c>
       <c r="M11" s="2">
-        <f>I11-E11</f>
+        <f t="shared" si="5"/>
         <v>2.5291595999999998</v>
       </c>
       <c r="N11" s="6">
-        <f>J11/F11</f>
+        <f t="shared" si="6"/>
         <v>0.15939703867107857</v>
       </c>
       <c r="O11" s="6">
-        <f>K11/G11</f>
+        <f t="shared" si="7"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="P11" s="6">
-        <f>N11-O11</f>
+        <f t="shared" si="8"/>
         <v>-1.7073549564215557E-2</v>
       </c>
     </row>
@@ -4014,15 +5543,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB528542-7572-41E1-B66C-DAA7120FD955}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B53" sqref="B2:B53"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>775</v>
       </c>
@@ -4032,8 +5561,11 @@
       <c r="C1" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1971</v>
       </c>
@@ -4043,8 +5575,12 @@
       <c r="C2" s="9">
         <v>46411700</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" t="e">
+        <f t="shared" ref="D2:D41" si="0">C2-C1</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>1972</v>
       </c>
@@ -4054,8 +5590,12 @@
       <c r="C3" s="9">
         <v>46571900</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>160200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>1973</v>
       </c>
@@ -4065,8 +5605,12 @@
       <c r="C4" s="9">
         <v>46686200</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>114300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>1974</v>
       </c>
@@ -4076,8 +5620,12 @@
       <c r="C5" s="9">
         <v>46682700</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-3500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>1975</v>
       </c>
@@ -4087,8 +5635,12 @@
       <c r="C6" s="9">
         <v>46674400</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-8300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>1976</v>
       </c>
@@ -4098,8 +5650,12 @@
       <c r="C7" s="9">
         <v>46659900</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-14500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>1977</v>
       </c>
@@ -4109,8 +5665,12 @@
       <c r="C8" s="9">
         <v>46639800</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-20100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>1978</v>
       </c>
@@ -4120,8 +5680,12 @@
       <c r="C9" s="9">
         <v>46638200</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>1979</v>
       </c>
@@ -4131,8 +5695,12 @@
       <c r="C10" s="9">
         <v>46698100</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>59900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>1980</v>
       </c>
@@ -4142,8 +5710,12 @@
       <c r="C11" s="9">
         <v>46787200</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>89100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>1981</v>
       </c>
@@ -4153,8 +5725,12 @@
       <c r="C12" s="9">
         <v>46820800</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>33600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>1982</v>
       </c>
@@ -4164,8 +5740,12 @@
       <c r="C13" s="9">
         <v>46777300</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-43500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>1983</v>
       </c>
@@ -4175,8 +5755,12 @@
       <c r="C14" s="9">
         <v>46813700</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>36400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>1984</v>
       </c>
@@ -4186,8 +5770,12 @@
       <c r="C15" s="9">
         <v>46912400</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>98700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>1985</v>
       </c>
@@ -4197,8 +5785,12 @@
       <c r="C16" s="9">
         <v>47057400</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>145000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>1986</v>
       </c>
@@ -4208,8 +5800,12 @@
       <c r="C17" s="9">
         <v>47187600</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>130200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>1987</v>
       </c>
@@ -4219,8 +5815,12 @@
       <c r="C18" s="9">
         <v>47300400</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>112800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>1988</v>
       </c>
@@ -4230,8 +5830,12 @@
       <c r="C19" s="9">
         <v>47412300</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>111900</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>1989</v>
       </c>
@@ -4241,8 +5845,12 @@
       <c r="C20" s="9">
         <v>47552700</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>140400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>1990</v>
       </c>
@@ -4252,8 +5860,12 @@
       <c r="C21" s="9">
         <v>47699100</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>146400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>1991</v>
       </c>
@@ -4263,8 +5875,12 @@
       <c r="C22" s="9">
         <v>47875000</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>175900</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>1992</v>
       </c>
@@ -4274,8 +5890,12 @@
       <c r="C23" s="9">
         <v>47998000</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>123000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>1993</v>
       </c>
@@ -4285,8 +5905,12 @@
       <c r="C24" s="9">
         <v>48102300</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>104300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>1994</v>
       </c>
@@ -4296,8 +5920,12 @@
       <c r="C25" s="9">
         <v>48228800</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>126500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="7">
         <v>1995</v>
       </c>
@@ -4307,8 +5935,12 @@
       <c r="C26" s="9">
         <v>48383500</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>154700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>1996</v>
       </c>
@@ -4318,8 +5950,12 @@
       <c r="C27" s="9">
         <v>48519100</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>135600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>1997</v>
       </c>
@@ -4329,8 +5965,12 @@
       <c r="C28" s="9">
         <v>48664800</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>145700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>1998</v>
       </c>
@@ -4340,8 +5980,12 @@
       <c r="C29" s="9">
         <v>48820600</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>155800</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="7">
         <v>1999</v>
       </c>
@@ -4351,8 +5995,12 @@
       <c r="C30" s="9">
         <v>49032900</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>212300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
         <v>2000</v>
       </c>
@@ -4362,8 +6010,12 @@
       <c r="C31" s="9">
         <v>49233300</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>200400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="7">
         <v>2001</v>
       </c>
@@ -4373,8 +6025,12 @@
       <c r="C32" s="9">
         <v>49449700</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>216400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="7">
         <v>2002</v>
       </c>
@@ -4384,8 +6040,12 @@
       <c r="C33" s="9">
         <v>49679300</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>229600</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="7">
         <v>2003</v>
       </c>
@@ -4395,8 +6055,12 @@
       <c r="C34" s="9">
         <v>49925500</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>246200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="7">
         <v>2004</v>
       </c>
@@ -4406,8 +6070,12 @@
       <c r="C35" s="9">
         <v>50194600</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>269100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="7">
         <v>2005</v>
       </c>
@@ -4417,8 +6085,12 @@
       <c r="C36" s="9">
         <v>50606000</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>411400</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
         <v>2006</v>
       </c>
@@ -4428,8 +6100,12 @@
       <c r="C37" s="9">
         <v>50965200</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>359200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="7">
         <v>2007</v>
       </c>
@@ -4439,8 +6115,12 @@
       <c r="C38" s="9">
         <v>51381100</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>415900</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="7">
         <v>2008</v>
       </c>
@@ -4450,8 +6130,12 @@
       <c r="C39" s="9">
         <v>51815900</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>434800</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="7">
         <v>2009</v>
       </c>
@@ -4461,8 +6145,12 @@
       <c r="C40" s="9">
         <v>52196400</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>380500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
         <v>2010</v>
       </c>
@@ -4472,8 +6160,12 @@
       <c r="C41" s="9">
         <v>52642500</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>446100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="7">
         <v>2011</v>
       </c>
@@ -4483,8 +6175,12 @@
       <c r="C42" s="9">
         <v>53107200</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D42">
+        <f t="shared" ref="D42:D52" si="1">C42-C41</f>
+        <v>464700</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="7">
         <v>2012</v>
       </c>
@@ -4494,8 +6190,12 @@
       <c r="C43" s="9">
         <v>53506800</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>399600</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="7">
         <v>2013</v>
       </c>
@@ -4505,8 +6205,12 @@
       <c r="C44" s="9">
         <v>53918700</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>411900</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
         <v>2014</v>
       </c>
@@ -4516,8 +6220,12 @@
       <c r="C45" s="9">
         <v>54370300</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>451600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="7">
         <v>2015</v>
       </c>
@@ -4527,8 +6235,12 @@
       <c r="C46" s="9">
         <v>54808700</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>438400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="7">
         <v>2016</v>
       </c>
@@ -4538,8 +6250,12 @@
       <c r="C47" s="9">
         <v>55289000</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>480300</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="7">
         <v>2017</v>
       </c>
@@ -4549,8 +6265,12 @@
       <c r="C48" s="9">
         <v>55619500</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>330500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="7">
         <v>2018</v>
       </c>
@@ -4560,8 +6280,12 @@
       <c r="C49" s="9">
         <v>55924500</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>305000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="7">
         <v>2019</v>
       </c>
@@ -4571,8 +6295,12 @@
       <c r="C50" s="9">
         <v>56230100</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>305600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="10">
         <v>2020</v>
       </c>
@@ -4582,8 +6310,12 @@
       <c r="C51" s="9">
         <v>56326000</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>95900</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="7">
         <v>2021</v>
       </c>
@@ -4593,8 +6325,12 @@
       <c r="C52" s="9">
         <v>56554900</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>228900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="11">
         <v>2022</v>
       </c>
@@ -4604,9 +6340,14 @@
       <c r="C53" s="9">
         <v>57106400</v>
       </c>
+      <c r="D53">
+        <f>C53-C52</f>
+        <v>551500</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18033,23 +19774,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f61fc314-c1ef-4837-abb9-2cec5da21052" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA951F4E0B9FE641B23975EA4A2B8210" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8a148f585abf6e078d51020145a4d2d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f61fc314-c1ef-4837-abb9-2cec5da21052" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e4d519de9a48b4b6f1fa662535f79c8b" ns3:_="">
     <xsd:import namespace="f61fc314-c1ef-4837-abb9-2cec5da21052"/>
@@ -18231,31 +19955,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617D293C-1F86-4899-8A16-DE7A89953A47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f61fc314-c1ef-4837-abb9-2cec5da21052"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{802BFD4E-800A-41AD-B662-7B4D42452EE8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f61fc314-c1ef-4837-abb9-2cec5da21052" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E113C5D0-1065-453A-B7A7-3A67DF5153C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18271,4 +19988,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{802BFD4E-800A-41AD-B662-7B4D42452EE8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{617D293C-1F86-4899-8A16-DE7A89953A47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f61fc314-c1ef-4837-abb9-2cec5da21052"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>